<commit_message>
Se concluido la primera parte del reporte el cual incluye la creación de los modelos, validacón cruzada y la información del corpus actualizado
</commit_message>
<xml_diff>
--- a/Desarrollo/Clasificador/Resultados/Prueba.08.10.2019/Reporte/Graficas/GraficaRecoleecion.xlsx
+++ b/Desarrollo/Clasificador/Resultados/Prueba.08.10.2019/Reporte/Graficas/GraficaRecoleecion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andrew/Documents/ESCOM/TT2/TT2/Desarrollo/Clasificador/Resultados/Prueba.08.10.2019/Reporte/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andrew/Documents/ESCOM/TT2/TT2/Desarrollo/Clasificador/Resultados/Prueba.08.10.2019/Reporte/Graficas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F33BBEB-7D6C-A841-BB8C-29BA2D791D17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A480D29-306F-404E-9D90-2A4ED4EA176A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{A6691E8A-B295-AE49-AFAE-55920EB11DBC}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{A6691E8A-B295-AE49-AFAE-55920EB11DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Recoleción" sheetId="1" r:id="rId1"/>
@@ -96,6 +96,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF004C91"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -128,19 +133,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1920" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
+                <a:effectLst/>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -148,13 +148,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>RESULTADOS</a:t>
+              <a:t>RESULTADOS DE RECCOLECIÓN</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> DE RECCOLECIÓN</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -171,19 +166,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1920" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -215,44 +205,73 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:srgbClr val="004C91"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
+              <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Recoleción!$A$3:$A$7</c:f>
@@ -307,15 +326,15 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
+        <c:gapWidth val="41"/>
         <c:axId val="792059919"/>
         <c:axId val="791923375"/>
       </c:barChart>
@@ -332,14 +351,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -350,10 +363,12 @@
             <a:pPr>
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst/>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -374,22 +389,8 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -397,10 +398,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -410,13 +412,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>NUMERO</a:t>
+                  <a:t>NUMERO DE NOTICIAS</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> DE NOTICIAS</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -433,10 +430,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -452,32 +450,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="792059919"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -491,9 +463,9 @@
           <a:noFill/>
           <a:ln w="9525">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
           </a:ln>
@@ -506,8 +478,9 @@
             <a:pPr rtl="0">
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -542,25 +515,28 @@
     <a:gradFill flip="none" rotWithShape="1">
       <a:gsLst>
         <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="68000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="85000"/>
           </a:schemeClr>
         </a:gs>
         <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="lt1"/>
         </a:gs>
       </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
+      <a:lin ang="5400000" scaled="1"/>
       <a:tileRect/>
     </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -610,19 +586,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1920" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -646,44 +617,73 @@
             <c:v>Noticias filtradas</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:srgbClr val="004C91"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
+              <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Filtro!$A$4:$A$8</c:f>
@@ -738,15 +738,15 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
+        <c:gapWidth val="41"/>
         <c:axId val="668904143"/>
         <c:axId val="769460623"/>
       </c:barChart>
@@ -763,14 +763,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -781,10 +775,12 @@
             <a:pPr>
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst/>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -805,22 +801,8 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -828,10 +810,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -859,10 +842,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -878,32 +862,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="668904143"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -917,9 +875,9 @@
           <a:noFill/>
           <a:ln w="9525">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
           </a:ln>
@@ -932,8 +890,9 @@
             <a:pPr rtl="0">
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -968,25 +927,28 @@
     <a:gradFill flip="none" rotWithShape="1">
       <a:gsLst>
         <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="68000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="85000"/>
           </a:schemeClr>
         </a:gs>
         <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
+          <a:schemeClr val="lt1"/>
         </a:gs>
       </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
+      <a:lin ang="5400000" scaled="1"/>
       <a:tileRect/>
     </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1089,83 +1051,8 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="204">
   <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1175,72 +1062,214 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200">
+      <a:effectLst/>
+    </cs:defRPr>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="68000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="84000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
   <cs:dataPointMarkerLayout symbol="circle" size="6"/>
@@ -1248,10 +1277,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1267,16 +1296,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1288,20 +1318,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1312,17 +1342,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1331,13 +1361,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1349,7 +1380,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -1357,14 +1388,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1376,14 +1407,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1394,17 +1425,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1413,14 +1444,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1431,8 +1462,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1442,7 +1474,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -1450,7 +1482,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1458,16 +1490,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1480,14 +1513,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1499,18 +1532,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+    <cs:defRPr kern="1200">
+      <a:effectLst/>
     </cs:defRPr>
   </cs:title>
   <cs:trendline>
@@ -1520,13 +1548,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1535,8 +1564,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1546,17 +1576,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1567,8 +1599,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1578,90 +1611,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="204">
   <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1671,72 +1629,214 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200">
+      <a:effectLst/>
+    </cs:defRPr>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="68000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="84000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="84000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
   <cs:dataPointMarkerLayout symbol="circle" size="6"/>
@@ -1744,10 +1844,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1763,16 +1863,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1784,20 +1885,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1808,17 +1909,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1827,13 +1928,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1845,7 +1947,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -1853,14 +1955,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1872,14 +1974,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1890,17 +1992,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1909,14 +2011,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1927,8 +2029,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1938,7 +2041,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -1946,7 +2049,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1954,16 +2057,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1976,14 +2080,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1995,18 +2099,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+    <cs:defRPr kern="1200">
+      <a:effectLst/>
     </cs:defRPr>
   </cs:title>
   <cs:trendline>
@@ -2016,13 +2115,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2031,8 +2131,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2042,17 +2143,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2063,8 +2166,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2074,7 +2178,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -2462,7 +2566,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2529,7 +2633,7 @@
   <dimension ref="A3:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>